<commit_message>
Versión 2.0.1 Adición de fotografías en archivo bruto, sin modificación de geojson
</commit_message>
<xml_diff>
--- a/assets/img/pacifico/inventory/continental/PACÍFICO_INVENTARIO.xlsx
+++ b/assets/img/pacifico/inventory/continental/PACÍFICO_INVENTARIO.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\Añadidos_litorales\assets\img\pacifico\inventory\continental\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Desarrollo_litorales\litorales\assets\img\pacifico\inventory\continental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EA6D8E-97B5-4EA4-86C7-2876F0D0D71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A598B1A-5986-4AC9-BD8C-A6805639E0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="128">
   <si>
     <t>Tumaco</t>
   </si>
@@ -306,12 +317,6 @@
     <t>Bahía de Tumaco, Mun. de Tumaco, Nariño. Por: Neider Aristizabal</t>
   </si>
   <si>
-    <t>/assets/img/pacifico/photos/continental/P_10.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/continental/P_10.jpeg</t>
-  </si>
-  <si>
     <t>Ensenada de Utria, Mun. de Bahía Solano, Chocó. Por: Liliana Sánchez Manco</t>
   </si>
   <si>
@@ -342,234 +347,6 @@
     <t>Playa del Bajito, Mun.de Tumaco, Nariño. Por: Daniela Alvarado Torrado</t>
   </si>
   <si>
-    <t>/assets/img/pacifico/photos/continental/P_2.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_3.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_4.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_5.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_6.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_7.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_8.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_9.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_11.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_12.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_13.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_14.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_15.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_16.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_17.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_18.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_19.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_20.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_21.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_23.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_24.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_25.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_26.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_27.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_28.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_29.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_30.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_31.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_32.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_33.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_34.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_35.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_36.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_37.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_38.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_39.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_40.jpeg</t>
-  </si>
-  <si>
-    <t>/assets/img/pacifico/photos/continental/P_41.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/continental/P_9.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/continental/P_8.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/continental/P_7.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/continental/P_6.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/continental/P_5.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/continental/P_4.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/continental/P_3.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/continental/P_2.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/continental/P_11.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_12.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_13.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_14.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_15.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_16.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_17.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_18.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_19.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_20.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_21.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_23.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_24.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_25.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_26.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_27.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_28.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_29.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_30.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_31.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_32.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_33.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_34.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_35.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_36.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_37.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_38.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_39.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_40.jpeg</t>
-  </si>
-  <si>
-    <t>https://github.com/litocol/litorales/tree/assets/img/pacifico/photos/continental/P_41.jpeg</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -625,13 +402,31 @@
   </si>
   <si>
     <t>Continental Pacífico</t>
+  </si>
+  <si>
+    <t>P_1</t>
+  </si>
+  <si>
+    <t>Yorlenys Romaña Torres</t>
+  </si>
+  <si>
+    <t>Bahía de Tumaco, Mun. de Tumaco, Nariño. Por: Yorlenys Romaña Torres</t>
+  </si>
+  <si>
+    <t>P_42</t>
+  </si>
+  <si>
+    <t>David Alonso Vera Mancipe</t>
+  </si>
+  <si>
+    <t>Playa del Bajito, Mun.de Tumaco, Nariño. Por: David Alonso Vera Mancipe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -651,14 +446,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -668,7 +455,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -691,17 +478,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -710,9 +504,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -991,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1022,66 +819,66 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>198</v>
+        <v>120</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>197</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>196</v>
+        <v>118</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>195</v>
+        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>194</v>
+        <v>116</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>193</v>
+        <v>115</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>192</v>
+        <v>114</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>191</v>
+        <v>113</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>190</v>
+        <v>112</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>189</v>
+        <v>111</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>188</v>
+        <v>110</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>187</v>
+        <v>109</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>182</v>
+        <v>104</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>181</v>
+        <v>103</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>183</v>
+        <v>105</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>184</v>
+        <v>106</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>185</v>
+        <v>107</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>186</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1102,7 +899,7 @@
         <v>42</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>12</v>
@@ -1123,24 +920,26 @@
         <v>42</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>105</v>
+        <v>124</v>
+      </c>
+      <c r="R2" t="str">
+        <f>"https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/" &amp; O2 &amp; ".jpeg"</f>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_1.jpeg</v>
+      </c>
+      <c r="S2" s="1" t="str">
+        <f>"/assets/img/pacifico/photos/continental/" &amp; O2 &amp; ".jpeg"</f>
+        <v>/assets/img/pacifico/photos/continental/P_1.jpeg</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -1182,7 +981,7 @@
         <v>42</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>42</v>
@@ -1190,16 +989,18 @@
       <c r="Q3" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>106</v>
+      <c r="R3" t="str">
+        <f t="shared" ref="R3:R41" si="0">"https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/" &amp; O3 &amp; ".jpeg"</f>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_2.jpeg</v>
+      </c>
+      <c r="S3" s="1" t="str">
+        <f t="shared" ref="S3:S43" si="1">"/assets/img/pacifico/photos/continental/" &amp; O3 &amp; ".jpeg"</f>
+        <v>/assets/img/pacifico/photos/continental/P_2.jpeg</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
@@ -1241,7 +1042,7 @@
         <v>42</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>42</v>
@@ -1249,16 +1050,18 @@
       <c r="Q4" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>107</v>
+      <c r="R4" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_3.jpeg</v>
+      </c>
+      <c r="S4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_3.jpeg</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -1300,7 +1103,7 @@
         <v>42</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>42</v>
@@ -1308,16 +1111,18 @@
       <c r="Q5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>108</v>
+      <c r="R5" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_4.jpeg</v>
+      </c>
+      <c r="S5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_4.jpeg</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -1359,7 +1164,7 @@
         <v>42</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>42</v>
@@ -1367,16 +1172,18 @@
       <c r="Q6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R6" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>109</v>
+      <c r="R6" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_5.jpeg</v>
+      </c>
+      <c r="S6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_5.jpeg</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -1418,7 +1225,7 @@
         <v>42</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>42</v>
@@ -1426,16 +1233,18 @@
       <c r="Q7" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R7" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>110</v>
+      <c r="R7" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_6.jpeg</v>
+      </c>
+      <c r="S7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_6.jpeg</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
@@ -1477,7 +1286,7 @@
         <v>42</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>42</v>
@@ -1485,16 +1294,18 @@
       <c r="Q8" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>111</v>
+      <c r="R8" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_7.jpeg</v>
+      </c>
+      <c r="S8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_7.jpeg</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -1536,7 +1347,7 @@
         <v>42</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>42</v>
@@ -1544,16 +1355,18 @@
       <c r="Q9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R9" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>112</v>
+      <c r="R9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_8.jpeg</v>
+      </c>
+      <c r="S9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_8.jpeg</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -1595,7 +1408,7 @@
         <v>42</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>42</v>
@@ -1603,16 +1416,18 @@
       <c r="Q10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R10" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>93</v>
+      <c r="R10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_9.jpeg</v>
+      </c>
+      <c r="S10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_9.jpeg</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
@@ -1654,7 +1469,7 @@
         <v>42</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>42</v>
@@ -1662,16 +1477,18 @@
       <c r="Q11" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R11" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>113</v>
+      <c r="R11" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_10.jpeg</v>
+      </c>
+      <c r="S11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_10.jpeg</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
@@ -1713,7 +1530,7 @@
         <v>42</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>42</v>
@@ -1721,16 +1538,18 @@
       <c r="Q12" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R12" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>114</v>
+      <c r="R12" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_11.jpeg</v>
+      </c>
+      <c r="S12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_11.jpeg</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1</v>
@@ -1772,7 +1591,7 @@
         <v>42</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>42</v>
@@ -1780,16 +1599,18 @@
       <c r="Q13" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R13" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>115</v>
+      <c r="R13" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_12.jpeg</v>
+      </c>
+      <c r="S13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_12.jpeg</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -1831,7 +1652,7 @@
         <v>42</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>42</v>
@@ -1839,93 +1660,97 @@
       <c r="Q14" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="R14" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>116</v>
+      <c r="R14" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_13.jpeg</v>
+      </c>
+      <c r="S14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_13.jpeg</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>117</v>
+        <v>92</v>
+      </c>
+      <c r="R15" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_14.jpeg</v>
+      </c>
+      <c r="S15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_14.jpeg</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>13</v>
@@ -1934,39 +1759,41 @@
         <v>12</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>20</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P16" s="3">
-        <v>44997</v>
+        <v>35</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="S16" s="1" t="s">
-        <v>118</v>
+        <v>93</v>
+      </c>
+      <c r="R16" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_15.jpeg</v>
+      </c>
+      <c r="S16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_15.jpeg</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>4</v>
@@ -1978,13 +1805,13 @@
         <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>13</v>
@@ -1996,7 +1823,7 @@
         <v>17</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>12</v>
@@ -2005,27 +1832,29 @@
         <v>20</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P17" s="3">
+        <v>36</v>
+      </c>
+      <c r="P17" s="2">
         <v>44997</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>119</v>
+        <v>94</v>
+      </c>
+      <c r="R17" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_16.jpeg</v>
+      </c>
+      <c r="S17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_16.jpeg</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>4</v>
@@ -2040,7 +1869,7 @@
         <v>47</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>44</v>
@@ -2067,45 +1896,47 @@
         <v>44</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P18" s="3">
+        <v>37</v>
+      </c>
+      <c r="P18" s="2">
         <v>44997</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>120</v>
+        <v>94</v>
+      </c>
+      <c r="R18" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_17.jpeg</v>
+      </c>
+      <c r="S18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_17.jpeg</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>12</v>
@@ -2117,33 +1948,35 @@
         <v>12</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="P19" s="2">
+        <v>44997</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="R19" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>121</v>
+        <v>94</v>
+      </c>
+      <c r="R19" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_18.jpeg</v>
+      </c>
+      <c r="S19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_18.jpeg</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>1</v>
@@ -2152,13 +1985,13 @@
         <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>44</v>
@@ -2179,48 +2012,50 @@
         <v>19</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>44</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>122</v>
+        <v>95</v>
+      </c>
+      <c r="R20" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_19.jpeg</v>
+      </c>
+      <c r="S20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_19.jpeg</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>54</v>
@@ -2235,54 +2070,56 @@
         <v>12</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>123</v>
+        <v>96</v>
+      </c>
+      <c r="R21" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_20.jpeg</v>
+      </c>
+      <c r="S21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_20.jpeg</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>12</v>
@@ -2300,27 +2137,29 @@
         <v>20</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>123</v>
+        <v>97</v>
+      </c>
+      <c r="R22" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_21.jpeg</v>
+      </c>
+      <c r="S22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_21.jpeg</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>4</v>
@@ -2362,24 +2201,26 @@
         <v>79</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>124</v>
+        <v>98</v>
+      </c>
+      <c r="R23" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_22.jpeg</v>
+      </c>
+      <c r="S23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_22.jpeg</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>4</v>
@@ -2421,24 +2262,26 @@
         <v>79</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="R24" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>125</v>
+        <v>98</v>
+      </c>
+      <c r="R24" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_23.jpeg</v>
+      </c>
+      <c r="S24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_23.jpeg</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>4</v>
@@ -2480,48 +2323,50 @@
         <v>79</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="R25" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>126</v>
+        <v>98</v>
+      </c>
+      <c r="R25" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_24.jpeg</v>
+      </c>
+      <c r="S25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_24.jpeg</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>77</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>17</v>
@@ -2536,51 +2381,53 @@
         <v>20</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="S26" s="1" t="s">
-        <v>127</v>
+        <v>98</v>
+      </c>
+      <c r="R26" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_25.jpeg</v>
+      </c>
+      <c r="S26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_25.jpeg</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>49</v>
+        <v>80</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>17</v>
@@ -2595,42 +2442,44 @@
         <v>20</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>128</v>
+        <v>99</v>
+      </c>
+      <c r="R27" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_26.jpeg</v>
+      </c>
+      <c r="S27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_26.jpeg</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>86</v>
@@ -2654,27 +2503,29 @@
         <v>20</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>129</v>
+        <v>100</v>
+      </c>
+      <c r="R28" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_27.jpeg</v>
+      </c>
+      <c r="S28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_27.jpeg</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>42</v>
@@ -2716,24 +2567,26 @@
         <v>42</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R29" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="S29" s="1" t="s">
-        <v>130</v>
+        <v>101</v>
+      </c>
+      <c r="R29" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_28.jpeg</v>
+      </c>
+      <c r="S29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_28.jpeg</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>42</v>
@@ -2775,24 +2628,26 @@
         <v>42</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R30" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="S30" s="1" t="s">
-        <v>131</v>
+        <v>101</v>
+      </c>
+      <c r="R30" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_29.jpeg</v>
+      </c>
+      <c r="S30" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_29.jpeg</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>42</v>
@@ -2834,24 +2689,26 @@
         <v>42</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R31" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>132</v>
+        <v>101</v>
+      </c>
+      <c r="R31" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_30.jpeg</v>
+      </c>
+      <c r="S31" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_30.jpeg</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>42</v>
@@ -2893,24 +2750,26 @@
         <v>42</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P32" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R32" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="S32" s="1" t="s">
-        <v>133</v>
+        <v>101</v>
+      </c>
+      <c r="R32" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_31.jpeg</v>
+      </c>
+      <c r="S32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_31.jpeg</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>42</v>
@@ -2952,24 +2811,26 @@
         <v>42</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R33" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="S33" s="1" t="s">
-        <v>134</v>
+        <v>101</v>
+      </c>
+      <c r="R33" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_32.jpeg</v>
+      </c>
+      <c r="S33" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_32.jpeg</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>42</v>
@@ -3011,24 +2872,26 @@
         <v>42</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P34" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R34" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="S34" s="1" t="s">
-        <v>135</v>
+        <v>101</v>
+      </c>
+      <c r="R34" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_33.jpeg</v>
+      </c>
+      <c r="S34" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_33.jpeg</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>42</v>
@@ -3070,24 +2933,26 @@
         <v>42</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P35" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R35" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="S35" s="1" t="s">
-        <v>136</v>
+        <v>101</v>
+      </c>
+      <c r="R35" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_34.jpeg</v>
+      </c>
+      <c r="S35" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_34.jpeg</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>42</v>
@@ -3129,24 +2994,26 @@
         <v>42</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P36" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R36" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="S36" s="1" t="s">
-        <v>137</v>
+        <v>101</v>
+      </c>
+      <c r="R36" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_35.jpeg</v>
+      </c>
+      <c r="S36" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_35.jpeg</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>42</v>
@@ -3188,24 +3055,26 @@
         <v>42</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P37" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R37" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="S37" s="1" t="s">
-        <v>138</v>
+        <v>101</v>
+      </c>
+      <c r="R37" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_36.jpeg</v>
+      </c>
+      <c r="S37" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_36.jpeg</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>42</v>
@@ -3247,24 +3116,26 @@
         <v>42</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R38" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="S38" s="1" t="s">
-        <v>139</v>
+        <v>101</v>
+      </c>
+      <c r="R38" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_37.jpeg</v>
+      </c>
+      <c r="S38" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_37.jpeg</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>42</v>
@@ -3306,45 +3177,47 @@
         <v>42</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P39" s="1" t="s">
         <v>42</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="R39" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="S39" s="1" t="s">
-        <v>140</v>
+        <v>101</v>
+      </c>
+      <c r="R39" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_38.jpeg</v>
+      </c>
+      <c r="S39" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_38.jpeg</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>12</v>
@@ -3356,33 +3229,35 @@
         <v>12</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="M40" s="1" t="s">
         <v>20</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P40" s="3">
-        <v>44397</v>
+        <v>72</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="R40" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="S40" s="1" t="s">
-        <v>141</v>
+        <v>101</v>
+      </c>
+      <c r="R40" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_39.jpeg</v>
+      </c>
+      <c r="S40" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_39.jpeg</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>1</v>
@@ -3415,75 +3290,157 @@
         <v>12</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>44</v>
       </c>
       <c r="O41" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P41" s="2">
+        <v>44397</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R41" t="str">
+        <f t="shared" si="0"/>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_40.jpeg</v>
+      </c>
+      <c r="S41" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_40.jpeg</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O42" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="P41" s="3">
+      <c r="P42" s="2">
         <v>44396</v>
       </c>
-      <c r="Q41" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="R41" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="S41" s="1" t="s">
-        <v>142</v>
+      <c r="Q42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R42" t="str">
+        <f>"https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/" &amp; O42 &amp; ".jpeg"</f>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_41.jpeg</v>
+      </c>
+      <c r="S42" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_41.jpeg</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="P43" s="5">
+        <v>45251</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R43" t="str">
+        <f>"https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/" &amp; O43 &amp; ".jpeg"</f>
+        <v>https://github.com/litocol/litorales/tree/main/assets/img/pacifico/photos/insular/P_42.jpeg</v>
+      </c>
+      <c r="S43" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>/assets/img/pacifico/photos/continental/P_42.jpeg</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="R10" r:id="rId1" xr:uid="{755ACA1E-E0A0-40BB-8166-FAC27DA0F30B}"/>
-    <hyperlink ref="R9" r:id="rId2" xr:uid="{5794B999-91B0-4142-9D1F-F3186B1FDA84}"/>
-    <hyperlink ref="R8" r:id="rId3" xr:uid="{ECCD105C-FE82-425F-85CA-14B7A6B96036}"/>
-    <hyperlink ref="R7" r:id="rId4" xr:uid="{A6DEECA2-CE53-4DD1-BA49-111E54493B2E}"/>
-    <hyperlink ref="R6" r:id="rId5" xr:uid="{9BE4521D-5F24-496D-8115-CA475ED48613}"/>
-    <hyperlink ref="R5" r:id="rId6" xr:uid="{83EFC76C-0163-4DB8-AD0F-8507DF272DAC}"/>
-    <hyperlink ref="R4" r:id="rId7" xr:uid="{9354CD47-23C2-44FF-AE07-0FEDEF387F76}"/>
-    <hyperlink ref="R3" r:id="rId8" xr:uid="{BBC1E2BF-C973-4D67-BE20-AFB6646CA718}"/>
-    <hyperlink ref="R2" r:id="rId9" xr:uid="{44A26FC7-B988-490E-92FA-62440984E9C1}"/>
-    <hyperlink ref="R11" r:id="rId10" xr:uid="{AA3F0BBD-ED72-4150-B8BE-D49706506299}"/>
-    <hyperlink ref="R12" r:id="rId11" xr:uid="{BCB71022-4DD5-46D1-B0E4-739E11C82DB3}"/>
-    <hyperlink ref="R13" r:id="rId12" xr:uid="{C7D1370B-C445-4812-8FE3-B173ABD819FF}"/>
-    <hyperlink ref="R14" r:id="rId13" xr:uid="{77F0E5B5-1B23-477D-BFC1-887BF4326C5C}"/>
-    <hyperlink ref="R15" r:id="rId14" xr:uid="{70B443FE-2A67-4FE8-9E48-27FC81499D61}"/>
-    <hyperlink ref="R16" r:id="rId15" xr:uid="{D3351295-555A-4CFE-A73D-2FD732A18FC1}"/>
-    <hyperlink ref="R17" r:id="rId16" xr:uid="{1BB9EB73-65A5-4CA5-84F2-A8312A2E0E18}"/>
-    <hyperlink ref="R18" r:id="rId17" xr:uid="{48BA6212-7005-4B8A-AC1A-370859F482F7}"/>
-    <hyperlink ref="R19" r:id="rId18" xr:uid="{7FE74E87-89BC-488B-96F4-221130514A8B}"/>
-    <hyperlink ref="R20" r:id="rId19" xr:uid="{223DF8C8-4824-495A-A6CB-08C1327C8024}"/>
-    <hyperlink ref="R21" r:id="rId20" xr:uid="{29E402C9-6007-4E99-BA6D-AEFC46677865}"/>
-    <hyperlink ref="R22" r:id="rId21" xr:uid="{86DB2B5C-5785-47FF-857F-8876A2EF73FF}"/>
-    <hyperlink ref="R23" r:id="rId22" xr:uid="{D02D20B8-F44E-45DE-A343-B4D61F2D5994}"/>
-    <hyperlink ref="R24" r:id="rId23" xr:uid="{3E3F7C99-9284-4E9D-98DE-4EF6ABB0EC3E}"/>
-    <hyperlink ref="R25" r:id="rId24" xr:uid="{4213AC5E-BF92-4322-8DDA-4A53F131A577}"/>
-    <hyperlink ref="R26" r:id="rId25" xr:uid="{ADFF0ABF-BFBC-4CEE-AB88-B2C9130C7187}"/>
-    <hyperlink ref="R27" r:id="rId26" xr:uid="{668BD00C-C0F1-42B0-975E-D69A3BB05CC9}"/>
-    <hyperlink ref="R28" r:id="rId27" xr:uid="{57FEC00D-E5F0-40F2-AF2B-C40F2AA2FC38}"/>
-    <hyperlink ref="R29" r:id="rId28" xr:uid="{ECDA0745-064A-4B40-AF8C-97A1FD043C46}"/>
-    <hyperlink ref="R30" r:id="rId29" xr:uid="{E236E061-59AD-41C7-BDEC-8AD9B63585C7}"/>
-    <hyperlink ref="R31" r:id="rId30" xr:uid="{956A41F3-88E6-4392-B0CA-77EA9CA19982}"/>
-    <hyperlink ref="R32" r:id="rId31" xr:uid="{3C35D91A-ED09-4144-94F7-ED44B11F2BF4}"/>
-    <hyperlink ref="R33" r:id="rId32" xr:uid="{E2DEF1AD-BA93-45F4-AE9E-DB43825E351C}"/>
-    <hyperlink ref="R34" r:id="rId33" xr:uid="{1E45E24A-C7AB-4D74-9F05-7D4A1067123F}"/>
-    <hyperlink ref="R35" r:id="rId34" xr:uid="{2AA19306-C73E-45A1-AD15-1EBA98774725}"/>
-    <hyperlink ref="R36" r:id="rId35" xr:uid="{062FC2E1-9921-4904-B96B-15AA1F411357}"/>
-    <hyperlink ref="R37" r:id="rId36" xr:uid="{66B323B1-939B-49A5-AB69-8FE7D5E23DCC}"/>
-    <hyperlink ref="R38" r:id="rId37" xr:uid="{09FB1408-1413-4DD0-A2A9-F835E960CF87}"/>
-    <hyperlink ref="R39" r:id="rId38" xr:uid="{B8DA888A-9D4F-4A49-8BFC-7FB22954AA17}"/>
-    <hyperlink ref="R40" r:id="rId39" xr:uid="{D1FC663D-9CE0-4EC9-B7EE-BE270CEA9E88}"/>
-    <hyperlink ref="R41" r:id="rId40" xr:uid="{D619628D-B9F6-4502-9451-D78686B87C3E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId41"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>